<commit_message>
NAV-128 fix test data spreadsheet resource reference
</commit_message>
<xml_diff>
--- a/navigator_engine/tests/test_data/Estimates_Navigator_BDG_Validations.xlsx
+++ b/navigator_engine/tests/test_data/Estimates_Navigator_BDG_Validations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soppe\Documents\Projects\navigator_engine\navigator_engine\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B39EDD-2AF5-4C09-9F03-9429DB1D2EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39374916-D885-4F57-A146-03581BAB14A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1452" yWindow="1536" windowWidth="20052" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="4392" windowWidth="20052" windowHeight="9312" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="00-Oveview" sheetId="1" r:id="rId1"/>
@@ -617,9 +617,6 @@
 Can easily remove.</t>
   </si>
   <si>
-    <t>check_resource_key(['inputs-unaids-geographic', 'inputs-unaids-survey', 'inputs-unaids-population', 'inputs-unaids-spectrum'], 'url', '.*')</t>
-  </si>
-  <si>
     <t>ADR-01-11</t>
   </si>
   <si>
@@ -979,6 +976,9 @@
   </si>
   <si>
     <t>check_manual_confirmation('EST-ROB-06-01-A')</t>
+  </si>
+  <si>
+    <t>check_resource_key(['inputs-unaids-geographic', 'inputs-unaids-survey', 'inputs-unaids-population', 'inputs-unaids-spectrum-file'], 'url', '.*')</t>
   </si>
 </sst>
 </file>
@@ -1639,9 +1639,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X995"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8121,9 +8121,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9663,7 +9663,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y996"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9770,28 +9772,28 @@
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="15" t="s">
-        <v>106</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="C6" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="D6" s="48" t="s">
         <v>109</v>
-      </c>
-      <c r="D6" s="48" t="s">
-        <v>110</v>
       </c>
       <c r="E6" s="32"/>
       <c r="F6" s="34"/>
       <c r="G6" s="49"/>
       <c r="H6" s="16"/>
       <c r="I6" s="50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J6" s="51"/>
       <c r="K6" s="51"/>
@@ -9812,16 +9814,16 @@
     </row>
     <row r="7" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="C7" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="D7" s="46" t="s">
         <v>114</v>
-      </c>
-      <c r="D7" s="46" t="s">
-        <v>115</v>
       </c>
       <c r="E7" s="32"/>
       <c r="F7" s="34">
@@ -9830,7 +9832,7 @@
       <c r="G7" s="49"/>
       <c r="H7" s="16"/>
       <c r="I7" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J7" s="51"/>
       <c r="K7" s="51"/>
@@ -9851,19 +9853,19 @@
     </row>
     <row r="8" spans="1:25" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="C8" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="D8" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="E8" s="37" t="s">
         <v>120</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>121</v>
       </c>
       <c r="F8" s="34">
         <v>1</v>
@@ -9871,7 +9873,7 @@
       <c r="G8" s="32"/>
       <c r="H8" s="16"/>
       <c r="I8" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -9892,19 +9894,19 @@
     </row>
     <row r="9" spans="1:25" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="C9" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="D9" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="E9" s="37" t="s">
         <v>126</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>127</v>
       </c>
       <c r="F9" s="34">
         <v>1</v>
@@ -9912,7 +9914,7 @@
       <c r="G9" s="32"/>
       <c r="H9" s="16"/>
       <c r="I9" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -9933,19 +9935,19 @@
     </row>
     <row r="10" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="54" t="s">
         <v>129</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="C10" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="D10" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="E10" s="55" t="s">
         <v>132</v>
-      </c>
-      <c r="E10" s="55" t="s">
-        <v>133</v>
       </c>
       <c r="F10" s="56">
         <v>1</v>
@@ -9953,7 +9955,7 @@
       <c r="G10" s="57"/>
       <c r="H10" s="58"/>
       <c r="I10" s="59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -9974,19 +9976,19 @@
     </row>
     <row r="11" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="C11" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="D11" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="E11" s="37" t="s">
         <v>138</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>139</v>
       </c>
       <c r="F11" s="32">
         <v>1</v>
@@ -9994,7 +9996,7 @@
       <c r="G11" s="32"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J11" s="60"/>
       <c r="K11" s="60"/>
@@ -11053,14 +11055,14 @@
     </row>
     <row r="2" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="75" t="s">
         <v>141</v>
-      </c>
-      <c r="B2" s="75" t="s">
-        <v>142</v>
       </c>
       <c r="C2" s="72"/>
       <c r="D2" s="75" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E2" s="72"/>
       <c r="F2" s="25">
@@ -11107,11 +11109,11 @@
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B5" s="62"/>
       <c r="C5" s="63" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D5" s="62"/>
       <c r="E5" s="62"/>
@@ -11119,28 +11121,28 @@
         <v>1</v>
       </c>
       <c r="G5" s="65" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H5" s="66"/>
       <c r="I5" s="67" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="D6" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="E6" s="13" t="s">
         <v>151</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>152</v>
       </c>
       <c r="F6" s="68">
         <v>1</v>
@@ -11148,21 +11150,21 @@
       <c r="G6" s="69"/>
       <c r="H6" s="13"/>
       <c r="I6" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="C7" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="D7" s="13" t="s">
         <v>156</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>157</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="68">
@@ -11171,21 +11173,21 @@
       <c r="G7" s="69"/>
       <c r="H7" s="13"/>
       <c r="I7" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="C8" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="D8" s="13" t="s">
         <v>161</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>162</v>
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="68">
@@ -11194,21 +11196,21 @@
       <c r="G8" s="69"/>
       <c r="H8" s="13"/>
       <c r="I8" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="C9" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="D9" s="32" t="s">
         <v>166</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>167</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>81</v>
@@ -11219,21 +11221,21 @@
       <c r="G9" s="69"/>
       <c r="H9" s="13"/>
       <c r="I9" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="C10" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="D10" s="32" t="s">
         <v>171</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>172</v>
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="69">
@@ -11242,7 +11244,7 @@
       <c r="G10" s="70"/>
       <c r="H10" s="19"/>
       <c r="I10" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>